<commit_message>
Cutscenes Main 03 ajustadas, 07 até 10 traduzidas e subm 01 e 02 traduzidas.
</commit_message>
<xml_diff>
--- a/Excel/auth_64/main/03/s03/cmn.xlsx
+++ b/Excel/auth_64/main/03/s03/cmn.xlsx
@@ -64,7 +64,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="3">
+  <fonts count="2">
     <font>
       <sz val="11.0"/>
       <color rgb="FF000000"/>
@@ -74,7 +74,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
     </font>
-    <font/>
   </fonts>
   <fills count="2">
     <fill>
@@ -90,14 +89,11 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -314,7 +310,10 @@
   </sheetViews>
   <sheetFormatPr customHeight="1" defaultColWidth="14.43" defaultRowHeight="15.0"/>
   <cols>
-    <col customWidth="1" min="1" max="26" width="8.71"/>
+    <col customWidth="1" min="1" max="1" width="8.71"/>
+    <col customWidth="1" min="2" max="2" width="41.43"/>
+    <col customWidth="1" min="3" max="3" width="42.43"/>
+    <col customWidth="1" min="4" max="26" width="8.71"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -335,7 +334,7 @@
       <c r="B2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="1" t="s">
         <v>4</v>
       </c>
     </row>
@@ -346,7 +345,7 @@
       <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -357,7 +356,7 @@
       <c r="B4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="1" t="s">
         <v>8</v>
       </c>
     </row>
@@ -368,7 +367,7 @@
       <c r="B5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -379,7 +378,7 @@
       <c r="B6" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="1" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>